<commit_message>
Add EditPartyList logic: supports updating party list name, renaming image folder, and saving new image to nested "Group Image" directory
</commit_message>
<xml_diff>
--- a/Modules.xlsx
+++ b/Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\GLP.Basecode.API.Voting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8128A45D-4B8C-4B0A-965B-677622D1BC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93800B7A-6C24-4E38-965C-D5D4BBF71671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{631B70AB-E6AF-41D8-A199-357B3A98B252}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Modules</t>
   </si>
@@ -252,12 +252,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402DA261-852C-4A23-BAFF-35C124DBF4B2}">
   <dimension ref="A2:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:P9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,10 +596,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -629,23 +629,23 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -653,64 +653,64 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -719,23 +719,23 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="5" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -743,22 +743,22 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -767,64 +767,64 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -833,43 +833,43 @@
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -878,43 +878,43 @@
       <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -923,23 +923,23 @@
       <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="5" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -947,22 +947,25 @@
       <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -971,64 +974,64 @@
       <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1037,22 +1040,22 @@
       <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1061,152 +1064,138 @@
       <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C29:P29"/>
-    <mergeCell ref="C30:P30"/>
-    <mergeCell ref="C31:P31"/>
-    <mergeCell ref="C23:P23"/>
-    <mergeCell ref="C24:P24"/>
-    <mergeCell ref="C25:P25"/>
-    <mergeCell ref="C26:P26"/>
-    <mergeCell ref="C27:P27"/>
-    <mergeCell ref="C28:P28"/>
-    <mergeCell ref="C17:P17"/>
-    <mergeCell ref="C19:P19"/>
-    <mergeCell ref="C18:P18"/>
-    <mergeCell ref="C20:P20"/>
-    <mergeCell ref="C21:P21"/>
     <mergeCell ref="C22:P22"/>
     <mergeCell ref="C14:P14"/>
     <mergeCell ref="C4:P4"/>
@@ -1221,6 +1210,20 @@
     <mergeCell ref="C8:P8"/>
     <mergeCell ref="C6:P6"/>
     <mergeCell ref="C5:P5"/>
+    <mergeCell ref="C17:P17"/>
+    <mergeCell ref="C19:P19"/>
+    <mergeCell ref="C18:P18"/>
+    <mergeCell ref="C20:P20"/>
+    <mergeCell ref="C21:P21"/>
+    <mergeCell ref="C29:P29"/>
+    <mergeCell ref="C30:P30"/>
+    <mergeCell ref="C31:P31"/>
+    <mergeCell ref="C23:P23"/>
+    <mergeCell ref="C24:P24"/>
+    <mergeCell ref="C25:P25"/>
+    <mergeCell ref="C26:P26"/>
+    <mergeCell ref="C27:P27"/>
+    <mergeCell ref="C28:P28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>